<commit_message>
2022-10-28 Alma R Viz workshop
</commit_message>
<xml_diff>
--- a/LessonMaterials/R/AlmaMaterials/sim_data.xlsx
+++ b/LessonMaterials/R/AlmaMaterials/sim_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/almaparada/Documents/CarpentryWorkshop/20221020_Rintro_Pt1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/almaparada/Documents/CarpentryWorkshop/20221028_Rintro_Pt2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C0D851-3BC2-324F-90AB-D59438D4E268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEC9A7F-4594-DC4F-892E-05BC89D3C3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="460" windowWidth="28040" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sim_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="111">
   <si>
     <t>S001</t>
   </si>
@@ -361,6 +361,12 @@
   </si>
   <si>
     <t>NO3_nanoM</t>
+  </si>
+  <si>
+    <t>Bact</t>
+  </si>
+  <si>
+    <t>Virus</t>
   </si>
 </sst>
 </file>
@@ -1201,15 +1207,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C101"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -1219,8 +1223,14 @@
       <c r="C1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1230,8 +1240,14 @@
       <c r="C2">
         <v>516.81764494870004</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>3210498</v>
+      </c>
+      <c r="E2">
+        <v>35013025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1241,8 +1257,14 @@
       <c r="C3">
         <v>435.04036563048197</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>3607997</v>
+      </c>
+      <c r="E3">
+        <v>36342384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1252,8 +1274,14 @@
       <c r="C4">
         <v>458.502165038653</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>3393192</v>
+      </c>
+      <c r="E4">
+        <v>37485073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1263,8 +1291,14 @@
       <c r="C5">
         <v>335.89332144104401</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>3316379</v>
+      </c>
+      <c r="E5">
+        <v>35002750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1274,8 +1308,14 @@
       <c r="C6">
         <v>401.321427825603</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>3759052</v>
+      </c>
+      <c r="E6">
+        <v>39974307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1285,8 +1325,14 @@
       <c r="C7">
         <v>367.33551554749499</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>3255187</v>
+      </c>
+      <c r="E7">
+        <v>33830160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1296,8 +1342,14 @@
       <c r="C8">
         <v>434.70552077825698</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>3976605</v>
+      </c>
+      <c r="E8">
+        <v>32538349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1307,8 +1359,14 @@
       <c r="C9">
         <v>424.76184113378702</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>3749163</v>
+      </c>
+      <c r="E9">
+        <v>38923467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1318,8 +1376,14 @@
       <c r="C10">
         <v>454.61458562252398</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>3538062</v>
+      </c>
+      <c r="E10">
+        <v>38681229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1329,8 +1393,14 @@
       <c r="C11">
         <v>414.41091674831199</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>3942572</v>
+      </c>
+      <c r="E11">
+        <v>37545017</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1340,8 +1410,14 @@
       <c r="C12">
         <v>494.59001128175697</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>3901402</v>
+      </c>
+      <c r="E12">
+        <v>31775960</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1351,8 +1427,14 @@
       <c r="C13">
         <v>396.75908365296499</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>3061941</v>
+      </c>
+      <c r="E13">
+        <v>35459129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1362,8 +1444,14 @@
       <c r="C14">
         <v>466.476280799047</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>2083545</v>
+      </c>
+      <c r="E14">
+        <v>24097683</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1373,8 +1461,14 @@
       <c r="C15">
         <v>511.61962640591997</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>3337790</v>
+      </c>
+      <c r="E15">
+        <v>22153322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1384,8 +1478,14 @@
       <c r="C16">
         <v>487.37668358085898</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>2970218</v>
+      </c>
+      <c r="E16">
+        <v>33026272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1395,8 +1495,14 @@
       <c r="C17">
         <v>373.2863444605</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>2032989</v>
+      </c>
+      <c r="E17">
+        <v>29732118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1406,8 +1512,14 @@
       <c r="C18">
         <v>436.60857324930902</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>2783023</v>
+      </c>
+      <c r="E18">
+        <v>25504624</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1417,8 +1529,14 @@
       <c r="C19">
         <v>494.62541410578302</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>2775446</v>
+      </c>
+      <c r="E19">
+        <v>34310173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1428,8 +1546,14 @@
       <c r="C20">
         <v>521.45233068068399</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>2463463</v>
+      </c>
+      <c r="E20">
+        <v>21088546</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1439,8 +1563,14 @@
       <c r="C21">
         <v>508.88799873456497</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>3183038</v>
+      </c>
+      <c r="E21">
+        <v>22719801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1450,8 +1580,14 @@
       <c r="C22">
         <v>327.297468909759</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>2484578</v>
+      </c>
+      <c r="E22">
+        <v>23423395</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1461,8 +1597,14 @@
       <c r="C23">
         <v>471.59401884951802</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>3380841</v>
+      </c>
+      <c r="E23">
+        <v>23919805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1472,8 +1614,14 @@
       <c r="C24">
         <v>488.77314322310201</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>3103813</v>
+      </c>
+      <c r="E24">
+        <v>31222139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1483,8 +1631,14 @@
       <c r="C25">
         <v>428.955145350821</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>2807591</v>
+      </c>
+      <c r="E25">
+        <v>20937942</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1494,8 +1648,14 @@
       <c r="C26">
         <v>501.90667088957298</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>2182982</v>
+      </c>
+      <c r="E26">
+        <v>26842766</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1505,8 +1665,14 @@
       <c r="C27">
         <v>418.26021962044302</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>2888132</v>
+      </c>
+      <c r="E27">
+        <v>21287895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1516,8 +1682,14 @@
       <c r="C28">
         <v>388.82710343246799</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>2211360</v>
+      </c>
+      <c r="E28">
+        <v>22315124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1527,8 +1699,14 @@
       <c r="C29">
         <v>411.64599421285601</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>3454525</v>
+      </c>
+      <c r="E29">
+        <v>20997689</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1538,8 +1716,14 @@
       <c r="C30">
         <v>457.54723953017998</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>3468694</v>
+      </c>
+      <c r="E30">
+        <v>25876883</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1549,8 +1733,14 @@
       <c r="C31">
         <v>415.34850136026103</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>3442447</v>
+      </c>
+      <c r="E31">
+        <v>26309250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1560,8 +1750,14 @@
       <c r="C32">
         <v>461.41334588694798</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>2813164</v>
+      </c>
+      <c r="E32">
+        <v>27041941</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1571,8 +1767,14 @@
       <c r="C33">
         <v>380.78870290496297</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>2229567</v>
+      </c>
+      <c r="E33">
+        <v>30821417</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1582,8 +1784,14 @@
       <c r="C34">
         <v>356.13466192849302</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>3277575</v>
+      </c>
+      <c r="E34">
+        <v>21590494</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1593,8 +1801,14 @@
       <c r="C35">
         <v>422.68296340661499</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>2185908</v>
+      </c>
+      <c r="E35">
+        <v>21620066</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1604,8 +1818,14 @@
       <c r="C36">
         <v>509.486561623559</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>2398769</v>
+      </c>
+      <c r="E36">
+        <v>26660702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1615,8 +1835,14 @@
       <c r="C37">
         <v>455.04220554506497</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>3023365</v>
+      </c>
+      <c r="E37">
+        <v>32996025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1626,8 +1852,14 @@
       <c r="C38">
         <v>432.45362389425497</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>2454216</v>
+      </c>
+      <c r="E38">
+        <v>26694425</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1637,8 +1869,14 @@
       <c r="C39">
         <v>486.72659901912101</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>2461136</v>
+      </c>
+      <c r="E39">
+        <v>28785131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1648,8 +1886,14 @@
       <c r="C40">
         <v>480.45775690496299</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>2827107</v>
+      </c>
+      <c r="E40">
+        <v>27918798</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1659,8 +1903,14 @@
       <c r="C41">
         <v>441.99003870996302</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>2979581</v>
+      </c>
+      <c r="E41">
+        <v>26218776</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1670,8 +1920,14 @@
       <c r="C42">
         <v>464.01550349237698</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>2042215</v>
+      </c>
+      <c r="E42">
+        <v>21771022</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1681,8 +1937,14 @@
       <c r="C43">
         <v>422.99890711975399</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>2765346</v>
+      </c>
+      <c r="E43">
+        <v>22269504</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1692,8 +1954,14 @@
       <c r="C44">
         <v>444.76270962019498</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>3142784</v>
+      </c>
+      <c r="E44">
+        <v>26493037</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1703,8 +1971,14 @@
       <c r="C45">
         <v>430.19672503985402</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>2135206</v>
+      </c>
+      <c r="E45">
+        <v>25167981</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1714,8 +1988,14 @@
       <c r="C46">
         <v>410.39278403792798</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>2359323</v>
+      </c>
+      <c r="E46">
+        <v>22749335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1725,8 +2005,14 @@
       <c r="C47">
         <v>437.91473296126298</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>2386795</v>
+      </c>
+      <c r="E47">
+        <v>24009172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1736,8 +2022,14 @@
       <c r="C48">
         <v>521.53326061781195</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>2822627</v>
+      </c>
+      <c r="E48">
+        <v>28427877</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1747,8 +2039,14 @@
       <c r="C49">
         <v>527.33325785237105</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>3131077</v>
+      </c>
+      <c r="E49">
+        <v>20215101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1758,8 +2056,14 @@
       <c r="C50">
         <v>440.03246772973898</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>2520093</v>
+      </c>
+      <c r="E50">
+        <v>31729370</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1769,8 +2073,14 @@
       <c r="C51">
         <v>460.02658326464501</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>2333276</v>
+      </c>
+      <c r="E51">
+        <v>25331638</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1780,8 +2090,14 @@
       <c r="C52">
         <v>2195.2146277697002</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>1838906</v>
+      </c>
+      <c r="E52">
+        <v>15464908</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1791,8 +2107,14 @@
       <c r="C53">
         <v>2166.5546312122146</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>2003335</v>
+      </c>
+      <c r="E53">
+        <v>17305626</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1802,8 +2124,14 @@
       <c r="C54">
         <v>2523.3184200676201</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>1586690</v>
+      </c>
+      <c r="E54">
+        <v>20223715</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1813,8 +2141,14 @@
       <c r="C55">
         <v>2845.4652738024947</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>1837862</v>
+      </c>
+      <c r="E55">
+        <v>16321134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1824,8 +2158,14 @@
       <c r="C56">
         <v>2236.3858980396199</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>1526989</v>
+      </c>
+      <c r="E56">
+        <v>23447263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1835,8 +2175,14 @@
       <c r="C57">
         <v>2965.8760808470652</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>1577734</v>
+      </c>
+      <c r="E57">
+        <v>15923241</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1846,8 +2192,14 @@
       <c r="C58">
         <v>2788.9499652918403</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>2231434</v>
+      </c>
+      <c r="E58">
+        <v>21082942</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1857,8 +2209,14 @@
       <c r="C59">
         <v>2991.9507679977</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>2268360</v>
+      </c>
+      <c r="E59">
+        <v>15723399</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1868,8 +2226,14 @@
       <c r="C60">
         <v>2902.0766777724998</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>2241985</v>
+      </c>
+      <c r="E60">
+        <v>16520904</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1879,8 +2243,14 @@
       <c r="C61">
         <v>3008.3470926152304</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>2437528</v>
+      </c>
+      <c r="E61">
+        <v>15981314</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1890,8 +2260,14 @@
       <c r="C62">
         <v>3212.7313466573296</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>2068383</v>
+      </c>
+      <c r="E62">
+        <v>18771839</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1901,8 +2277,14 @@
       <c r="C63">
         <v>3531.1587092102504</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>1615152</v>
+      </c>
+      <c r="E63">
+        <v>17761502</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1912,8 +2294,14 @@
       <c r="C64">
         <v>3143.4050826407547</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>2213315</v>
+      </c>
+      <c r="E64">
+        <v>24413358</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1923,8 +2311,14 @@
       <c r="C65">
         <v>2625.3957525545047</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>1660935</v>
+      </c>
+      <c r="E65">
+        <v>23732024</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1934,8 +2328,14 @@
       <c r="C66">
         <v>2779.8618229076851</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>1962698</v>
+      </c>
+      <c r="E66">
+        <v>23147831</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1945,8 +2345,14 @@
       <c r="C67">
         <v>3171.1254665438505</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>2322450</v>
+      </c>
+      <c r="E67">
+        <v>23384141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1956,8 +2362,14 @@
       <c r="C68">
         <v>2645.8297845880497</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>1614384</v>
+      </c>
+      <c r="E68">
+        <v>21647282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1967,8 +2379,14 @@
       <c r="C69">
         <v>3237.1314323627848</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>1562875</v>
+      </c>
+      <c r="E69">
+        <v>24249035</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1978,8 +2396,14 @@
       <c r="C70">
         <v>3360.3235743150899</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>2174848</v>
+      </c>
+      <c r="E70">
+        <v>20404423</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1989,8 +2413,14 @@
       <c r="C71">
         <v>2464.3056175033553</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>2236181</v>
+      </c>
+      <c r="E71">
+        <v>15238426</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2000,8 +2430,14 @@
       <c r="C72">
         <v>2905.2209433601597</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>1743841</v>
+      </c>
+      <c r="E72">
+        <v>20628353</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -2011,8 +2447,14 @@
       <c r="C73">
         <v>2947.3246167669599</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>1664482</v>
+      </c>
+      <c r="E73">
+        <v>15926605</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2022,8 +2464,14 @@
       <c r="C74">
         <v>3246.4448318693403</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>1747955</v>
+      </c>
+      <c r="E74">
+        <v>23987789</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2033,8 +2481,14 @@
       <c r="C75">
         <v>2651.3504790409547</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>1778322</v>
+      </c>
+      <c r="E75">
+        <v>22127750</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -2044,8 +2498,14 @@
       <c r="C76">
         <v>2848.755486418775</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>1736103</v>
+      </c>
+      <c r="E76">
+        <v>16303555</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2055,8 +2515,14 @@
       <c r="C77">
         <v>583.14946583901099</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <v>513553</v>
+      </c>
+      <c r="E77">
+        <v>6159722</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2066,8 +2532,14 @@
       <c r="C78">
         <v>662.975605224726</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <v>977632</v>
+      </c>
+      <c r="E78">
+        <v>6062956</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2077,8 +2549,14 @@
       <c r="C79">
         <v>649.46588816715405</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>660553</v>
+      </c>
+      <c r="E79">
+        <v>8637679</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2088,8 +2566,14 @@
       <c r="C80">
         <v>567.16103678535205</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>961959</v>
+      </c>
+      <c r="E80">
+        <v>9997966</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -2099,8 +2583,14 @@
       <c r="C81">
         <v>666.46984713037898</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>683661</v>
+      </c>
+      <c r="E81">
+        <v>8156532</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -2110,8 +2600,14 @@
       <c r="C82">
         <v>651.87117510351197</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <v>562710</v>
+      </c>
+      <c r="E82">
+        <v>6593136</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -2121,8 +2617,14 @@
       <c r="C83">
         <v>617.49230412300994</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>979649</v>
+      </c>
+      <c r="E83">
+        <v>5125780</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -2132,8 +2634,14 @@
       <c r="C84">
         <v>563.03892010510697</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>898494</v>
+      </c>
+      <c r="E84">
+        <v>8819204</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -2143,8 +2651,14 @@
       <c r="C85">
         <v>658.66124709379096</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>815554</v>
+      </c>
+      <c r="E85">
+        <v>6795263</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -2154,8 +2668,14 @@
       <c r="C86">
         <v>626.40602616052797</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>850447</v>
+      </c>
+      <c r="E86">
+        <v>7341379</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -2165,8 +2685,14 @@
       <c r="C87">
         <v>633.78837978537695</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <v>985542</v>
+      </c>
+      <c r="E87">
+        <v>9509600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -2176,8 +2702,14 @@
       <c r="C88">
         <v>635.94506148995094</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>645302</v>
+      </c>
+      <c r="E88">
+        <v>9766693</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -2187,8 +2719,14 @@
       <c r="C89">
         <v>582.77033067281502</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>627923</v>
+      </c>
+      <c r="E89">
+        <v>9351795</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -2198,8 +2736,14 @@
       <c r="C90">
         <v>555.21419333071901</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <v>831298</v>
+      </c>
+      <c r="E90">
+        <v>3032095</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -2209,8 +2753,14 @@
       <c r="C91">
         <v>644.56880293188306</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <v>811258</v>
+      </c>
+      <c r="E91">
+        <v>7855211</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2220,8 +2770,14 @@
       <c r="C92">
         <v>570.68412907061702</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <v>683041</v>
+      </c>
+      <c r="E92">
+        <v>8022944</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2231,8 +2787,14 @@
       <c r="C93">
         <v>579.64194744098995</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <v>851317</v>
+      </c>
+      <c r="E93">
+        <v>5489116</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -2242,8 +2804,14 @@
       <c r="C94">
         <v>692.25971636663303</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <v>322410</v>
+      </c>
+      <c r="E94">
+        <v>6954119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -2253,8 +2821,14 @@
       <c r="C95">
         <v>576.28958212590499</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <v>831148</v>
+      </c>
+      <c r="E95">
+        <v>9608943</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -2264,8 +2838,14 @@
       <c r="C96">
         <v>592.71358149327205</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <v>971441</v>
+      </c>
+      <c r="E96">
+        <v>6173843</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -2275,8 +2855,14 @@
       <c r="C97">
         <v>530.97256284629998</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <v>280554</v>
+      </c>
+      <c r="E97">
+        <v>3025182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -2286,8 +2872,14 @@
       <c r="C98">
         <v>555.91381275946299</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <v>800451</v>
+      </c>
+      <c r="E98">
+        <v>7561349</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2297,8 +2889,14 @@
       <c r="C99">
         <v>532.29102985142197</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <v>380976</v>
+      </c>
+      <c r="E99">
+        <v>4274743</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -2308,8 +2906,14 @@
       <c r="C100">
         <v>536.644903862609</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <v>710537</v>
+      </c>
+      <c r="E100">
+        <v>8951115</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -2318,6 +2922,12 @@
       </c>
       <c r="C101">
         <v>601.34423001304106</v>
+      </c>
+      <c r="D101">
+        <v>888011</v>
+      </c>
+      <c r="E101">
+        <v>2820997</v>
       </c>
     </row>
   </sheetData>
@@ -2332,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5885830D-9506-8244-9ED6-7F5DEAD06E25}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>